<commit_message>
ran flight_time.py and generated calculation logs
</commit_message>
<xml_diff>
--- a/einstein_550.xlsx
+++ b/einstein_550.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Timothy/Desktop/Projects/software/flybys_foci/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A6CA8D-EB30-1341-9629-45BBFE144A39}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE07F05-48D0-7E4A-ABA8-2E7D0190DA7E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="27920" windowHeight="17040" xr2:uid="{DD63909C-8122-8041-A566-2E7D9A3C8601}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="165" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +525,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="1">
-        <v>550</v>
+        <v>600</v>
       </c>
       <c r="C6" t="s">
         <v>6</v>

</xml_diff>